<commit_message>
Update artifacts and requirements stack
</commit_message>
<xml_diff>
--- a/Documentation/EECS 582 Requirements.xlsx
+++ b/Documentation/EECS 582 Requirements.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="65">
   <si>
     <t>REQUIREMENTS STACK:</t>
   </si>
@@ -52,37 +52,19 @@
     <t>Find text dataset to train model on</t>
   </si>
   <si>
-    <t>name teehee</t>
+    <t>Write Training Algorithm</t>
   </si>
   <si>
     <t>Train model on dataset</t>
   </si>
   <si>
-    <t>We have little reference for how long it will take to
-train model on datasets specific to our purposes,
-so it likely won't take 21 points, just a placeholder
-for uncertainty</t>
-  </si>
-  <si>
-    <t>objective</t>
-  </si>
-  <si>
     <t>Design output data format</t>
   </si>
   <si>
-    <t>novelty</t>
-  </si>
-  <si>
     <t>Image-&gt;alt-text intermediate step</t>
   </si>
   <si>
-    <t>last week</t>
-  </si>
-  <si>
     <t>Create text webscraper</t>
-  </si>
-  <si>
-    <t>next week</t>
   </si>
   <si>
     <t>Create image webscraper</t>
@@ -369,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -398,18 +380,12 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -753,12 +729,12 @@
         <v>1.0</v>
       </c>
       <c r="F3" s="8">
-        <f>SUM(C3:C7)</f>
+        <f>SUM(C3:C8)</f>
         <v>33</v>
       </c>
       <c r="H3" s="9">
-        <f>SUM(C3:C22)</f>
-        <v>155</v>
+        <f>SUM(C3:C23)</f>
+        <v>161</v>
       </c>
     </row>
     <row r="4">
@@ -796,98 +772,81 @@
         <v>1.0</v>
       </c>
       <c r="F5" s="8"/>
-      <c r="J5" s="4" t="s">
+    </row>
+    <row r="6">
+      <c r="A6" s="7">
+        <v>4.0</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="5">
-        <v>4.0</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="7">
+        <v>13.0</v>
+      </c>
+      <c r="D6" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="7">
-        <v>21.0</v>
-      </c>
-      <c r="D6" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="E6" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="4" t="s">
+      <c r="C7" s="7">
+        <v>8.0</v>
+      </c>
+      <c r="D7" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="7">
+        <v>6.0</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="5">
-        <v>5.0</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="D7" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="J7" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="11">
-        <v>6.0</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="12">
-        <v>5.0</v>
-      </c>
-      <c r="D8" s="13">
-        <v>1.0</v>
-      </c>
-      <c r="E8" s="12">
-        <v>2.0</v>
-      </c>
-      <c r="F8" s="14">
-        <f>SUM(C8:C14)</f>
-        <v>31</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="C8" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="D8" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="E8" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="F8" s="8"/>
     </row>
     <row r="9">
       <c r="A9" s="11">
         <v>7.0</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C9" s="12">
         <v>5.0</v>
       </c>
-      <c r="D9" s="13">
-        <v>2.0</v>
+      <c r="D9" s="11">
+        <v>1.0</v>
       </c>
       <c r="E9" s="12">
         <v>2.0</v>
       </c>
-      <c r="F9" s="14"/>
-      <c r="J9" s="4" t="s">
-        <v>21</v>
+      <c r="F9" s="13">
+        <f>SUM(C9:C15)</f>
+        <v>37</v>
       </c>
     </row>
     <row r="10">
@@ -895,233 +854,251 @@
         <v>8.0</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C10" s="12">
-        <v>5.0</v>
-      </c>
-      <c r="D10" s="13">
+        <v>8.0</v>
+      </c>
+      <c r="D10" s="11">
         <v>2.0</v>
       </c>
       <c r="E10" s="12">
         <v>2.0</v>
       </c>
-      <c r="F10" s="14"/>
+      <c r="F10" s="13"/>
     </row>
     <row r="11">
-      <c r="A11" s="15">
+      <c r="A11" s="11">
         <v>9.0</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C11" s="12">
-        <v>5.0</v>
-      </c>
-      <c r="D11" s="13">
+        <v>8.0</v>
+      </c>
+      <c r="D11" s="11">
         <v>2.0</v>
       </c>
       <c r="E11" s="12">
         <v>2.0</v>
       </c>
-      <c r="F11" s="14"/>
+      <c r="F11" s="13"/>
     </row>
     <row r="12">
       <c r="A12" s="11">
         <v>10.0</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C12" s="12">
         <v>5.0</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="11">
         <v>2.0</v>
       </c>
       <c r="E12" s="12">
         <v>2.0</v>
       </c>
-      <c r="F12" s="14"/>
-    </row>
-    <row r="13" ht="18.75" customHeight="1">
-      <c r="A13" s="13">
+      <c r="F12" s="13"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="11">
         <v>11.0</v>
       </c>
       <c r="B13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="12">
+        <v>5.0</v>
+      </c>
+      <c r="D13" s="11">
+        <v>2.0</v>
+      </c>
+      <c r="E13" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="F13" s="13"/>
+    </row>
+    <row r="14" ht="18.75" customHeight="1">
+      <c r="A14" s="11">
+        <v>12.0</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="D14" s="11">
+        <v>2.0</v>
+      </c>
+      <c r="E14" s="14">
+        <v>2.0</v>
+      </c>
+      <c r="F14" s="13"/>
+    </row>
+    <row r="15" ht="17.25" customHeight="1">
+      <c r="A15" s="11">
+        <v>13.0</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="D15" s="11">
+        <v>3.0</v>
+      </c>
+      <c r="E15" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="F15" s="13"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="15">
+        <v>14.0</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="16">
+        <v>2.0</v>
+      </c>
+      <c r="D16" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="E16" s="16">
+        <v>3.0</v>
+      </c>
+      <c r="F16" s="17">
+        <f>SUM(C16:C19)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="15">
+        <v>15.0</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="16">
+        <v>5.0</v>
+      </c>
+      <c r="D17" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="E17" s="16">
+        <v>3.0</v>
+      </c>
+      <c r="F17" s="17"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="15">
+        <v>16.0</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="16">
+        <v>8.0</v>
+      </c>
+      <c r="D18" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="E18" s="16">
+        <v>3.0</v>
+      </c>
+      <c r="F18" s="17"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="15">
+        <v>17.0</v>
+      </c>
+      <c r="B19" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="12">
-        <v>3.0</v>
-      </c>
-      <c r="D13" s="13">
-        <v>2.0</v>
-      </c>
-      <c r="E13" s="16">
-        <v>2.0</v>
-      </c>
-      <c r="F13" s="14"/>
-    </row>
-    <row r="14" ht="17.25" customHeight="1">
-      <c r="A14" s="13">
-        <v>12.0</v>
-      </c>
-      <c r="B14" s="16" t="s">
+      <c r="C19" s="16">
+        <v>13.0</v>
+      </c>
+      <c r="D19" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="E19" s="16">
+        <v>3.0</v>
+      </c>
+      <c r="F19" s="17"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="18">
+        <v>18.0</v>
+      </c>
+      <c r="B20" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="12">
-        <v>3.0</v>
-      </c>
-      <c r="D14" s="13">
-        <v>3.0</v>
-      </c>
-      <c r="E14" s="12">
-        <v>2.0</v>
-      </c>
-      <c r="F14" s="14"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="17">
-        <v>13.0</v>
-      </c>
-      <c r="B15" s="18" t="s">
+      <c r="C20" s="19">
+        <v>21.0</v>
+      </c>
+      <c r="D20" s="18">
+        <v>4.0</v>
+      </c>
+      <c r="E20" s="19">
+        <v>4.0</v>
+      </c>
+      <c r="F20" s="20"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="21">
+        <v>19.0</v>
+      </c>
+      <c r="B21" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="18">
-        <v>2.0</v>
-      </c>
-      <c r="D15" s="17">
-        <v>3.0</v>
-      </c>
-      <c r="E15" s="18">
-        <v>3.0</v>
-      </c>
-      <c r="F15" s="19">
-        <f>SUM(C15:C18)</f>
+      <c r="C21" s="23">
+        <v>21.0</v>
+      </c>
+      <c r="D21" s="21">
+        <v>4.0</v>
+      </c>
+      <c r="E21" s="23">
+        <v>5.0</v>
+      </c>
+      <c r="F21" s="24"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="25">
+        <v>20.0</v>
+      </c>
+      <c r="B22" s="26" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="17">
-        <v>14.0</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="18">
+      <c r="C22" s="27">
+        <v>21.0</v>
+      </c>
+      <c r="D22" s="25">
         <v>5.0</v>
       </c>
-      <c r="D16" s="17">
-        <v>3.0</v>
-      </c>
-      <c r="E16" s="18">
-        <v>3.0</v>
-      </c>
-      <c r="F16" s="19"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="17">
-        <v>15.0</v>
-      </c>
-      <c r="B17" s="18" t="s">
+      <c r="E22" s="26">
+        <v>6.0</v>
+      </c>
+      <c r="F22" s="28"/>
+      <c r="G22" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="18">
-        <v>8.0</v>
-      </c>
-      <c r="D17" s="17">
-        <v>3.0</v>
-      </c>
-      <c r="E17" s="18">
-        <v>3.0</v>
-      </c>
-      <c r="F17" s="19"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="17">
-        <v>16.0</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="18">
-        <v>13.0</v>
-      </c>
-      <c r="D18" s="17">
-        <v>3.0</v>
-      </c>
-      <c r="E18" s="18">
-        <v>3.0</v>
-      </c>
-      <c r="F18" s="19"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="20">
-        <v>17.0</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="21">
-        <v>21.0</v>
-      </c>
-      <c r="D19" s="20">
-        <v>4.0</v>
-      </c>
-      <c r="E19" s="21">
-        <v>4.0</v>
-      </c>
-      <c r="F19" s="22"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="23">
-        <v>18.0</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="25">
-        <v>21.0</v>
-      </c>
-      <c r="D20" s="23">
-        <v>4.0</v>
-      </c>
-      <c r="E20" s="25">
-        <v>5.0</v>
-      </c>
-      <c r="F20" s="26"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="27">
-        <v>19.0</v>
-      </c>
-      <c r="B21" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="29">
-        <v>21.0</v>
-      </c>
-      <c r="D21" s="27">
-        <v>5.0</v>
-      </c>
-      <c r="E21" s="28">
-        <v>6.0</v>
-      </c>
-      <c r="F21" s="30"/>
-      <c r="G21" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="31"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="32"/>
     </row>
     <row r="23">
-      <c r="A23" s="33"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="33"/>
+      <c r="A23" s="29"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="30"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="31"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="31"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1146,24 +1123,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3">
@@ -1174,13 +1151,13 @@
         <v>5.0</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="34" t="s">
-        <v>42</v>
+        <v>36</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>37</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F3" s="9">
         <f>COUNTIF(B3:B46,1)</f>
@@ -1195,13 +1172,13 @@
         <v>13.0</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="35" t="s">
-        <v>45</v>
+        <v>36</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>40</v>
       </c>
       <c r="F4" s="9">
         <f>COUNTIF(B3:B46,2)</f>
@@ -1216,13 +1193,13 @@
         <v>2.0</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="35" t="s">
-        <v>47</v>
+      <c r="E5" s="33" t="s">
+        <v>42</v>
       </c>
       <c r="F5" s="9">
         <f>COUNTIF(B3:B46,3)</f>
@@ -1237,13 +1214,13 @@
         <v>3.0</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="35" t="s">
-        <v>49</v>
+        <v>36</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>44</v>
       </c>
       <c r="F6" s="9">
         <f>COUNTIF(B3:B46,5)</f>
@@ -1258,13 +1235,13 @@
         <v>3.0</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="35" t="s">
-        <v>51</v>
+        <v>36</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>46</v>
       </c>
       <c r="F7" s="9">
         <f>COUNTIF(B3:B46,8)</f>
@@ -1279,15 +1256,15 @@
         <v>8.0</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="37">
+        <v>36</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="35">
         <f>COUNTIF(B3:B46,13)</f>
         <v>3</v>
       </c>
@@ -1300,10 +1277,10 @@
         <v>13.0</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="34" t="s">
-        <v>55</v>
+        <v>49</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>50</v>
       </c>
       <c r="F9" s="9">
         <f>COUNTIF(B3:B46,21)</f>
@@ -1318,10 +1295,10 @@
         <v>2.0</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="34" t="s">
-        <v>56</v>
+        <v>49</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="11">
@@ -1332,10 +1309,10 @@
         <v>3.0</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12">
@@ -1346,10 +1323,10 @@
         <v>5.0</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13">
@@ -1360,10 +1337,10 @@
         <v>8.0</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14">
@@ -1374,10 +1351,10 @@
         <v>5.0</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="38" t="s">
-        <v>60</v>
+        <v>36</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="15">
@@ -1388,10 +1365,10 @@
         <v>2.0</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16">
@@ -1402,10 +1379,10 @@
         <v>13.0</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17">
@@ -1416,10 +1393,10 @@
         <v>5.0</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18">
@@ -1430,10 +1407,10 @@
         <v>8.0</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19">
@@ -1444,10 +1421,10 @@
         <v>1.0</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20">
@@ -1458,10 +1435,10 @@
         <v>1.0</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="21">
@@ -1472,10 +1449,10 @@
         <v>8.0</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22">
@@ -1486,14 +1463,14 @@
         <v>1.0</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24">
-      <c r="E24" s="39"/>
+      <c r="E24" s="37"/>
     </row>
   </sheetData>
   <autoFilter ref="$B$3:$B$22"/>

</xml_diff>